<commit_message>
03: Progress in theory and experimental part
</commit_message>
<xml_diff>
--- a/03_PaschenuvZakon/data/PaschenuvZakon.xlsx
+++ b/03_PaschenuvZakon/data/PaschenuvZakon.xlsx
@@ -1,22 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Desktop\Škola Mgr\Praktikum plazma\PraktikaPlazma\03_PaschenuvZakon\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69A3ABC9-6F3D-4FC4-9198-90515AFE291E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="60" windowWidth="15315" windowHeight="11835"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="38">
   <si>
     <t>Tlak [Pa]</t>
   </si>
@@ -61,13 +79,85 @@
   </si>
   <si>
     <t>d[mm]</t>
+  </si>
+  <si>
+    <t>p*d</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>NewFunction (User)</t>
+  </si>
+  <si>
+    <t>Equation</t>
+  </si>
+  <si>
+    <t>B*x/(C+ln(x))</t>
+  </si>
+  <si>
+    <t>Plot</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>440,67861 ± 94,46346</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>1,68206 ± 0,02532</t>
+  </si>
+  <si>
+    <t>Reduced Chi-Sqr</t>
+  </si>
+  <si>
+    <t>R-Square (COD)</t>
+  </si>
+  <si>
+    <t>Adj. R-Square</t>
+  </si>
+  <si>
+    <t>286,26452 ± 27,21599</t>
+  </si>
+  <si>
+    <t>0,79493 ± 0,01431</t>
+  </si>
+  <si>
+    <t>U = f(I)</t>
+  </si>
+  <si>
+    <t>tlak 100 Pa</t>
+  </si>
+  <si>
+    <t>Proud [muA]</t>
+  </si>
+  <si>
+    <t>Odpor ohm</t>
+  </si>
+  <si>
+    <t>Proud A</t>
+  </si>
+  <si>
+    <t>U0 841</t>
+  </si>
+  <si>
+    <t>log I A</t>
+  </si>
+  <si>
+    <t>log I muA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="175" formatCode="0.00000000"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -76,16 +166,29 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -93,15 +196,110 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFC0C0C0"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFC0C0C0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFC0C0C0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFC0C0C0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFC0C0C0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFC0C0C0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFC0C0C0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -109,12 +307,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -156,7 +357,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -189,9 +390,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -224,6 +442,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -399,41 +634,104 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AE46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P32" sqref="P32"/>
+      <selection activeCell="X2" sqref="X2:X14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="14" width="5.7109375" customWidth="1"/>
+    <col min="24" max="24" width="15.42578125" customWidth="1"/>
+    <col min="25" max="25" width="13.7109375" customWidth="1"/>
+    <col min="28" max="28" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O1" t="s">
+        <v>2</v>
+      </c>
+      <c r="P1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R1" t="s">
+        <v>3</v>
+      </c>
+      <c r="U1" t="s">
+        <v>2</v>
+      </c>
+      <c r="V1" t="s">
+        <v>4</v>
+      </c>
+      <c r="W1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O2" t="s">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>33</v>
+      </c>
+      <c r="Q2">
+        <v>40</v>
+      </c>
+      <c r="R2">
+        <v>713</v>
+      </c>
+      <c r="U2" t="s">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>100</v>
+      </c>
+      <c r="W2">
+        <v>42</v>
+      </c>
+      <c r="X2">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3">
         <v>33</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q3">
+        <v>35</v>
+      </c>
+      <c r="R3">
+        <v>712</v>
+      </c>
+      <c r="W3">
+        <v>36</v>
+      </c>
+      <c r="X3">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>1</v>
       </c>
@@ -461,8 +759,20 @@
       <c r="J4">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q4">
+        <v>30</v>
+      </c>
+      <c r="R4">
+        <v>709</v>
+      </c>
+      <c r="W4">
+        <v>31</v>
+      </c>
+      <c r="X4">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -493,8 +803,20 @@
       <c r="J5">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q5">
+        <v>25</v>
+      </c>
+      <c r="R5">
+        <v>706</v>
+      </c>
+      <c r="W5">
+        <v>25</v>
+      </c>
+      <c r="X5">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -525,24 +847,74 @@
       <c r="J6">
         <v>737</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q6">
+        <v>20</v>
+      </c>
+      <c r="R6">
+        <v>701</v>
+      </c>
+      <c r="W6">
+        <v>20</v>
+      </c>
+      <c r="X6">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Q7">
+        <v>18</v>
+      </c>
+      <c r="R7">
+        <v>701</v>
+      </c>
+      <c r="W7">
+        <v>18</v>
+      </c>
+      <c r="X7">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
       <c r="B8" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q8">
+        <v>16</v>
+      </c>
+      <c r="R8">
+        <v>703</v>
+      </c>
+      <c r="W8">
+        <v>17</v>
+      </c>
+      <c r="X8">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>0</v>
       </c>
       <c r="B9">
         <v>100</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q9">
+        <v>15</v>
+      </c>
+      <c r="R9">
+        <v>728</v>
+      </c>
+      <c r="W9">
+        <v>16</v>
+      </c>
+      <c r="X9">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>1</v>
       </c>
@@ -582,8 +954,20 @@
       <c r="N10">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q10">
+        <v>14</v>
+      </c>
+      <c r="R10">
+        <v>737</v>
+      </c>
+      <c r="W10">
+        <v>15</v>
+      </c>
+      <c r="X10">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -626,8 +1010,14 @@
       <c r="N11">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="W11">
+        <v>14</v>
+      </c>
+      <c r="X11">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -670,8 +1060,30 @@
       <c r="N12">
         <v>550</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="W12">
+        <v>8</v>
+      </c>
+      <c r="X12">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="W13">
+        <v>7</v>
+      </c>
+      <c r="X13">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="W14">
+        <v>6</v>
+      </c>
+      <c r="X14">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -679,15 +1091,39 @@
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>7</v>
       </c>
       <c r="B17">
         <v>841</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="W17" t="s">
+        <v>30</v>
+      </c>
+      <c r="X17" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA17" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC17" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -724,8 +1160,44 @@
       <c r="L18">
         <v>30.02</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="V18" t="s">
+        <v>35</v>
+      </c>
+      <c r="W18" t="s">
+        <v>31</v>
+      </c>
+      <c r="X18">
+        <f>841-(Y18*Z18)</f>
+        <v>584.24</v>
+      </c>
+      <c r="Y18">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="Z18">
+        <v>2620</v>
+      </c>
+      <c r="AA18">
+        <f>Y18*1000000</f>
+        <v>98000</v>
+      </c>
+      <c r="AB18" s="7">
+        <f>Z18/1000000</f>
+        <v>2.6199999999999999E-3</v>
+      </c>
+      <c r="AC18">
+        <f>LOG10(AB18)</f>
+        <v>-2.5816987086802548</v>
+      </c>
+      <c r="AD18">
+        <f t="shared" ref="AD18:AD27" si="0">AC18/$AC$28</f>
+        <v>0.51788722499499462</v>
+      </c>
+      <c r="AE18">
+        <f>LOG10(Z18)</f>
+        <v>3.4183012913197452</v>
+      </c>
+    </row>
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -762,8 +1234,38 @@
       <c r="L19">
         <v>10</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="X19">
+        <f t="shared" ref="X19:X28" si="1">841-(Y19*Z19)</f>
+        <v>503.82799999999997</v>
+      </c>
+      <c r="Y19">
+        <v>0.316</v>
+      </c>
+      <c r="Z19">
+        <v>1067</v>
+      </c>
+      <c r="AA19">
+        <f t="shared" ref="AA19:AA28" si="2">Y19*1000000</f>
+        <v>316000</v>
+      </c>
+      <c r="AB19" s="7">
+        <f t="shared" ref="AB19:AB28" si="3">Z19/1000000</f>
+        <v>1.067E-3</v>
+      </c>
+      <c r="AC19">
+        <f t="shared" ref="AC19:AC28" si="4">LOG10(AB19)</f>
+        <v>-2.9718355805755299</v>
+      </c>
+      <c r="AD19">
+        <f t="shared" si="0"/>
+        <v>0.59614844938757938</v>
+      </c>
+      <c r="AE19">
+        <f t="shared" ref="AE19:AE28" si="5">LOG10(Z19)</f>
+        <v>3.0281644194244697</v>
+      </c>
+    </row>
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -797,8 +1299,38 @@
       <c r="L20">
         <v>11</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="X20">
+        <f t="shared" si="1"/>
+        <v>485.28199999999998</v>
+      </c>
+      <c r="Y20">
+        <v>0.874</v>
+      </c>
+      <c r="Z20">
+        <v>407</v>
+      </c>
+      <c r="AA20">
+        <f t="shared" si="2"/>
+        <v>874000</v>
+      </c>
+      <c r="AB20" s="7">
+        <f t="shared" si="3"/>
+        <v>4.0700000000000003E-4</v>
+      </c>
+      <c r="AC20">
+        <f t="shared" si="4"/>
+        <v>-3.3904055907747801</v>
+      </c>
+      <c r="AD20">
+        <f t="shared" si="0"/>
+        <v>0.68011334440781535</v>
+      </c>
+      <c r="AE20">
+        <f t="shared" si="5"/>
+        <v>2.6095944092252199</v>
+      </c>
+    </row>
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -823,8 +1355,38 @@
       <c r="L21">
         <v>11.8</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="X21">
+        <f t="shared" si="1"/>
+        <v>480.892</v>
+      </c>
+      <c r="Y21">
+        <v>1.429</v>
+      </c>
+      <c r="Z21">
+        <v>252</v>
+      </c>
+      <c r="AA21">
+        <f t="shared" si="2"/>
+        <v>1429000</v>
+      </c>
+      <c r="AB21" s="7">
+        <f t="shared" si="3"/>
+        <v>2.52E-4</v>
+      </c>
+      <c r="AC21">
+        <f t="shared" si="4"/>
+        <v>-3.5985994592184558</v>
+      </c>
+      <c r="AD21">
+        <f t="shared" si="0"/>
+        <v>0.72187691055391512</v>
+      </c>
+      <c r="AE21">
+        <f t="shared" si="5"/>
+        <v>2.4014005407815442</v>
+      </c>
+    </row>
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>11</v>
       </c>
@@ -837,67 +1399,353 @@
       <c r="L22">
         <v>10.35</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="X22">
+        <f>841-(Y22*Z22)</f>
+        <v>492.71080000000001</v>
+      </c>
+      <c r="Y22">
+        <v>1.897</v>
+      </c>
+      <c r="Z22">
+        <v>183.6</v>
+      </c>
+      <c r="AA22">
+        <f t="shared" si="2"/>
+        <v>1897000</v>
+      </c>
+      <c r="AB22" s="7">
+        <f t="shared" si="3"/>
+        <v>1.8359999999999999E-4</v>
+      </c>
+      <c r="AC22">
+        <f t="shared" si="4"/>
+        <v>-3.7361273231347765</v>
+      </c>
+      <c r="AD22">
+        <f t="shared" si="0"/>
+        <v>0.74946491823414574</v>
+      </c>
+      <c r="AE22">
+        <f t="shared" si="5"/>
+        <v>2.2638726768652235</v>
+      </c>
+    </row>
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="X23">
+        <f t="shared" si="1"/>
+        <v>499.77119999999996</v>
+      </c>
+      <c r="Y23">
+        <v>2.8820000000000001</v>
+      </c>
+      <c r="Z23">
+        <v>118.4</v>
+      </c>
+      <c r="AA23">
+        <f t="shared" si="2"/>
+        <v>2882000</v>
+      </c>
+      <c r="AB23" s="7">
+        <f t="shared" si="3"/>
+        <v>1.184E-4</v>
+      </c>
+      <c r="AC23">
+        <f t="shared" si="4"/>
+        <v>-3.9266482976130992</v>
+      </c>
+      <c r="AD23">
+        <f t="shared" si="0"/>
+        <v>0.78768331236517874</v>
+      </c>
+      <c r="AE23">
+        <f t="shared" si="5"/>
+        <v>2.0733517023869008</v>
+      </c>
+    </row>
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="X24">
+        <f t="shared" si="1"/>
+        <v>502.82379999999995</v>
+      </c>
+      <c r="Y24">
+        <v>4.8380000000000001</v>
+      </c>
+      <c r="Z24">
+        <v>69.900000000000006</v>
+      </c>
+      <c r="AA24">
+        <f t="shared" si="2"/>
+        <v>4838000</v>
+      </c>
+      <c r="AB24" s="7">
+        <f t="shared" si="3"/>
+        <v>6.9900000000000005E-5</v>
+      </c>
+      <c r="AC24">
+        <f t="shared" si="4"/>
+        <v>-4.1555228242543185</v>
+      </c>
+      <c r="AD24">
+        <f t="shared" si="0"/>
+        <v>0.83359540624187134</v>
+      </c>
+      <c r="AE24">
+        <f t="shared" si="5"/>
+        <v>1.8444771757456815</v>
+      </c>
+    </row>
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="N25" t="s">
+        <v>0</v>
+      </c>
+      <c r="O25">
+        <v>100</v>
+      </c>
+      <c r="R25" t="s">
+        <v>14</v>
+      </c>
+      <c r="S25">
+        <v>20</v>
+      </c>
+      <c r="X25">
+        <f t="shared" si="1"/>
+        <v>501.40999999999997</v>
+      </c>
+      <c r="Y25">
+        <v>11.71</v>
+      </c>
+      <c r="Z25">
+        <v>29</v>
+      </c>
+      <c r="AA25">
+        <f t="shared" si="2"/>
+        <v>11710000</v>
+      </c>
+      <c r="AB25" s="7">
+        <f t="shared" si="3"/>
+        <v>2.9E-5</v>
+      </c>
+      <c r="AC25">
+        <f t="shared" si="4"/>
+        <v>-4.5376020021010435</v>
+      </c>
+      <c r="AD25">
+        <f t="shared" si="0"/>
+        <v>0.91024026200219399</v>
+      </c>
+      <c r="AE25">
+        <f t="shared" si="5"/>
+        <v>1.4623979978989561</v>
+      </c>
+    </row>
+    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N26" t="s">
+        <v>14</v>
+      </c>
+      <c r="O26" t="s">
+        <v>7</v>
+      </c>
+      <c r="P26" t="s">
+        <v>15</v>
+      </c>
+      <c r="R26" t="s">
+        <v>0</v>
+      </c>
+      <c r="S26" t="s">
+        <v>7</v>
+      </c>
+      <c r="T26" t="s">
+        <v>15</v>
+      </c>
+      <c r="X26">
+        <f t="shared" si="1"/>
+        <v>551.43759999999997</v>
+      </c>
+      <c r="Y26">
+        <v>15.72</v>
+      </c>
+      <c r="Z26">
+        <v>18.420000000000002</v>
+      </c>
+      <c r="AA26">
+        <f t="shared" si="2"/>
+        <v>15720000</v>
+      </c>
+      <c r="AB26" s="7">
+        <f t="shared" si="3"/>
+        <v>1.8420000000000003E-5</v>
+      </c>
+      <c r="AC26">
+        <f t="shared" si="4"/>
+        <v>-4.7347103741391701</v>
+      </c>
+      <c r="AD26">
+        <f t="shared" si="0"/>
+        <v>0.9497800841645907</v>
+      </c>
+      <c r="AE26">
+        <f t="shared" si="5"/>
+        <v>1.2652896258608302</v>
+      </c>
+    </row>
+    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B27">
         <f>$B$28*B29/1000</f>
         <v>5</v>
       </c>
       <c r="C27">
-        <f t="shared" ref="C27:K27" si="0">$B$28*C29/1000</f>
+        <f>$B$28*C29/1000</f>
         <v>4</v>
       </c>
       <c r="D27">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D27:K27" si="6">$B$28*D29/1000</f>
         <v>3</v>
       </c>
       <c r="E27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>2.5</v>
       </c>
       <c r="F27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="G27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>1.5</v>
       </c>
       <c r="H27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>0.9</v>
       </c>
       <c r="J27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>0.7</v>
       </c>
       <c r="K27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>0.4</v>
       </c>
       <c r="L27">
         <f>$B$28*L29/1000</f>
         <v>0.2</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N27">
+        <v>50</v>
+      </c>
+      <c r="O27">
+        <v>450</v>
+      </c>
+      <c r="P27">
+        <f>N27*$B$28/1000</f>
+        <v>5</v>
+      </c>
+      <c r="R27">
+        <v>25</v>
+      </c>
+      <c r="S27">
+        <v>1360</v>
+      </c>
+      <c r="T27">
+        <f>R27*$B$33/1000</f>
+        <v>0.5</v>
+      </c>
+      <c r="X27">
+        <f t="shared" si="1"/>
+        <v>542.57119999999998</v>
+      </c>
+      <c r="Y27">
+        <v>20.84</v>
+      </c>
+      <c r="Z27">
+        <v>14.32</v>
+      </c>
+      <c r="AA27">
+        <f t="shared" si="2"/>
+        <v>20840000</v>
+      </c>
+      <c r="AB27" s="7">
+        <f t="shared" si="3"/>
+        <v>1.432E-5</v>
+      </c>
+      <c r="AC27">
+        <f t="shared" si="4"/>
+        <v>-4.8440569820281629</v>
+      </c>
+      <c r="AD27">
+        <f t="shared" si="0"/>
+        <v>0.9717149486520098</v>
+      </c>
+      <c r="AE27">
+        <f t="shared" si="5"/>
+        <v>1.1559430179718369</v>
+      </c>
+    </row>
+    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>0</v>
       </c>
       <c r="B28">
         <v>100</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N28">
+        <v>40</v>
+      </c>
+      <c r="O28">
+        <v>430</v>
+      </c>
+      <c r="P28">
+        <f t="shared" ref="P28:P37" si="7">N28*$B$28/1000</f>
+        <v>4</v>
+      </c>
+      <c r="R28">
+        <v>30</v>
+      </c>
+      <c r="S28">
+        <v>850</v>
+      </c>
+      <c r="T28">
+        <f t="shared" ref="T28:T37" si="8">R28*$B$33/1000</f>
+        <v>0.6</v>
+      </c>
+      <c r="X28">
+        <f t="shared" si="1"/>
+        <v>530.29300000000001</v>
+      </c>
+      <c r="Y28">
+        <v>30.02</v>
+      </c>
+      <c r="Z28">
+        <v>10.35</v>
+      </c>
+      <c r="AA28">
+        <f t="shared" si="2"/>
+        <v>30020000</v>
+      </c>
+      <c r="AB28" s="7">
+        <f t="shared" si="3"/>
+        <v>1.0349999999999999E-5</v>
+      </c>
+      <c r="AC28">
+        <f t="shared" si="4"/>
+        <v>-4.9850596502070639</v>
+      </c>
+      <c r="AD28">
+        <f>AC28/$AC$28</f>
+        <v>1</v>
+      </c>
+      <c r="AE28">
+        <f t="shared" si="5"/>
+        <v>1.0149403497929366</v>
+      </c>
+    </row>
+    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -934,8 +1782,28 @@
       <c r="L29">
         <v>2</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N29">
+        <v>30</v>
+      </c>
+      <c r="O29">
+        <v>390</v>
+      </c>
+      <c r="P29">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="R29">
+        <v>37</v>
+      </c>
+      <c r="S29">
+        <v>560</v>
+      </c>
+      <c r="T29">
+        <f t="shared" si="8"/>
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>7</v>
       </c>
@@ -972,62 +1840,144 @@
       <c r="L30">
         <v>1200</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N30">
+        <v>25</v>
+      </c>
+      <c r="O30">
+        <v>380</v>
+      </c>
+      <c r="P30">
+        <f t="shared" si="7"/>
+        <v>2.5</v>
+      </c>
+      <c r="R30">
+        <v>46</v>
+      </c>
+      <c r="S30">
+        <v>460</v>
+      </c>
+      <c r="T30">
+        <f t="shared" si="8"/>
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="N31">
+        <v>20</v>
+      </c>
+      <c r="O31">
+        <v>360</v>
+      </c>
+      <c r="P31">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="R31">
+        <v>58</v>
+      </c>
+      <c r="S31">
+        <v>410</v>
+      </c>
+      <c r="T31">
+        <f t="shared" si="8"/>
+        <v>1.1599999999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B32">
         <f>$B$33*B34/1000</f>
         <v>0.5</v>
       </c>
       <c r="C32">
-        <f t="shared" ref="C32:L32" si="1">$B$33*C34/1000</f>
+        <f t="shared" ref="C32:L32" si="9">$B$33*C34/1000</f>
         <v>0.6</v>
       </c>
       <c r="D32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>0.74</v>
       </c>
       <c r="E32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>0.92</v>
       </c>
       <c r="F32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>1.1599999999999999</v>
       </c>
       <c r="G32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>1.34</v>
       </c>
       <c r="H32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>1.6</v>
       </c>
       <c r="I32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="J32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
       <c r="K32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>4.4000000000000004</v>
       </c>
       <c r="L32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N32">
+        <v>15</v>
+      </c>
+      <c r="O32">
+        <v>370</v>
+      </c>
+      <c r="P32">
+        <f t="shared" si="7"/>
+        <v>1.5</v>
+      </c>
+      <c r="R32">
+        <v>67</v>
+      </c>
+      <c r="S32">
+        <v>380</v>
+      </c>
+      <c r="T32">
+        <f t="shared" si="8"/>
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>14</v>
       </c>
       <c r="B33">
         <v>20</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N33">
+        <v>10</v>
+      </c>
+      <c r="O33">
+        <v>400</v>
+      </c>
+      <c r="P33">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="R33">
+        <v>80</v>
+      </c>
+      <c r="S33">
+        <v>370</v>
+      </c>
+      <c r="T33">
+        <f t="shared" si="8"/>
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>0</v>
       </c>
@@ -1064,8 +2014,28 @@
       <c r="L34">
         <v>300</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N34">
+        <v>9</v>
+      </c>
+      <c r="O34">
+        <v>440</v>
+      </c>
+      <c r="P34">
+        <f t="shared" si="7"/>
+        <v>0.9</v>
+      </c>
+      <c r="R34">
+        <v>100</v>
+      </c>
+      <c r="S34">
+        <v>360</v>
+      </c>
+      <c r="T34">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>7</v>
       </c>
@@ -1102,14 +2072,191 @@
       <c r="L35">
         <v>530</v>
       </c>
+      <c r="N35">
+        <v>7</v>
+      </c>
+      <c r="O35">
+        <v>470</v>
+      </c>
+      <c r="P35">
+        <f t="shared" si="7"/>
+        <v>0.7</v>
+      </c>
+      <c r="R35">
+        <v>150</v>
+      </c>
+      <c r="S35">
+        <v>380</v>
+      </c>
+      <c r="T35">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="N36">
+        <v>4</v>
+      </c>
+      <c r="O36">
+        <v>900</v>
+      </c>
+      <c r="P36">
+        <f t="shared" si="7"/>
+        <v>0.4</v>
+      </c>
+      <c r="R36">
+        <v>220</v>
+      </c>
+      <c r="S36">
+        <v>420</v>
+      </c>
+      <c r="T36">
+        <f t="shared" si="8"/>
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="N37">
+        <v>2</v>
+      </c>
+      <c r="O37">
+        <v>1200</v>
+      </c>
+      <c r="P37">
+        <f t="shared" si="7"/>
+        <v>0.2</v>
+      </c>
+      <c r="R37">
+        <v>300</v>
+      </c>
+      <c r="S37">
+        <v>530</v>
+      </c>
+      <c r="T37">
+        <f t="shared" si="8"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" ht="24" x14ac:dyDescent="0.25">
+      <c r="N39" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O39" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="R39" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S39" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" ht="24" x14ac:dyDescent="0.25">
+      <c r="N40" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="O40" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="R40" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="S40" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="N41" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O41" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="R41" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="S41" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+      <c r="N42" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O42" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="R42" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="S42" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" ht="24" x14ac:dyDescent="0.25">
+      <c r="N43" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O43" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="R43" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="S43" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" ht="48" x14ac:dyDescent="0.25">
+      <c r="N44" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="O44" s="4">
+        <v>71212.206839999999</v>
+      </c>
+      <c r="R44" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="S44" s="4">
+        <v>14837.657440000001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" ht="60" x14ac:dyDescent="0.25">
+      <c r="N45" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="O45" s="4">
+        <v>0.11873</v>
+      </c>
+      <c r="R45" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="S45" s="4">
+        <v>0.85443999999999998</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+      <c r="N46" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="O46" s="6">
+        <v>2.0809999999999999E-2</v>
+      </c>
+      <c r="R46" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="S46" s="6">
+        <v>0.83826999999999996</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1121,7 +2268,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
03: Correct graphs and fits
</commit_message>
<xml_diff>
--- a/03_PaschenuvZakon/data/PaschenuvZakon.xlsx
+++ b/03_PaschenuvZakon/data/PaschenuvZakon.xlsx
@@ -1,17 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Desktop\Škola Mgr\Praktikum plazma\PraktikaPlazma\03_PaschenuvZakon\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{504E85C8-9CAB-4706-9D1D-3C3CB8F4E2E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="19176"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -96,15 +102,9 @@
     <t>B</t>
   </si>
   <si>
-    <t>440,67861 ± 94,46346</t>
-  </si>
-  <si>
     <t>C</t>
   </si>
   <si>
-    <t>1,68206 ± 0,02532</t>
-  </si>
-  <si>
     <t>Reduced Chi-Sqr</t>
   </si>
   <si>
@@ -142,12 +142,18 @@
   </si>
   <si>
     <t>log I muA</t>
+  </si>
+  <si>
+    <t>306,53892 ± 29,21135</t>
+  </si>
+  <si>
+    <t>1,0501 ± 0,02154</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00000000"/>
   </numFmts>
@@ -293,7 +299,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -309,7 +315,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -351,7 +357,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -384,9 +390,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -419,6 +442,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -594,25 +634,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB30" sqref="AB30"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="U45" sqref="U45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="14" width="5.6640625" customWidth="1"/>
-    <col min="24" max="24" width="15.44140625" customWidth="1"/>
-    <col min="25" max="25" width="13.6640625" customWidth="1"/>
-    <col min="26" max="26" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="14" width="5.7109375" customWidth="1"/>
+    <col min="24" max="24" width="15.42578125" customWidth="1"/>
+    <col min="25" max="25" width="13.7109375" customWidth="1"/>
+    <col min="26" max="26" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -641,7 +681,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -673,7 +713,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -693,7 +733,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="4" spans="1:24" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>1</v>
       </c>
@@ -734,7 +774,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="5" spans="1:24" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -778,7 +818,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="6" spans="1:24" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -822,7 +862,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="7" spans="1:24" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="Q7">
         <v>18</v>
       </c>
@@ -836,7 +876,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="8" spans="1:24" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -856,7 +896,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="9" spans="1:24" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -876,7 +916,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="10" spans="1:24" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>1</v>
       </c>
@@ -929,7 +969,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="11" spans="1:24" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -979,7 +1019,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="12" spans="1:24" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -1029,7 +1069,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="13" spans="1:24" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="W13">
         <v>7</v>
       </c>
@@ -1037,7 +1077,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="14" spans="1:24" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="W14">
         <v>6</v>
       </c>
@@ -1045,7 +1085,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="16" spans="1:24" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -1053,7 +1093,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -1061,7 +1101,7 @@
         <v>841</v>
       </c>
       <c r="W17" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="X17" t="s">
         <v>7</v>
@@ -1070,22 +1110,22 @@
         <v>6</v>
       </c>
       <c r="Z17" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA17" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB17" t="s">
         <v>32</v>
       </c>
-      <c r="AA17" t="s">
-        <v>33</v>
-      </c>
-      <c r="AB17" t="s">
+      <c r="AC17" t="s">
         <v>34</v>
       </c>
-      <c r="AC17" t="s">
-        <v>36</v>
-      </c>
       <c r="AE17" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -1123,10 +1163,10 @@
         <v>30.02</v>
       </c>
       <c r="V18" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="W18" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="X18">
         <f>841-(Y18*Z18)</f>
@@ -1159,7 +1199,7 @@
         <v>3.4183012913197452</v>
       </c>
     </row>
-    <row r="19" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -1227,7 +1267,7 @@
         <v>3.0115704435972783</v>
       </c>
     </row>
-    <row r="20" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -1292,7 +1332,7 @@
         <v>2.6095944092252199</v>
       </c>
     </row>
-    <row r="21" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -1348,7 +1388,7 @@
         <v>2.4014005407815442</v>
       </c>
     </row>
-    <row r="22" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>11</v>
       </c>
@@ -1392,7 +1432,7 @@
         <v>2.2638726768652235</v>
       </c>
     </row>
-    <row r="23" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="X23">
         <f t="shared" si="1"/>
         <v>499.77119999999996</v>
@@ -1424,7 +1464,7 @@
         <v>2.0733517023869008</v>
       </c>
     </row>
-    <row r="24" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="X24">
         <f t="shared" si="1"/>
         <v>502.82379999999995</v>
@@ -1456,7 +1496,7 @@
         <v>1.8444771757456815</v>
       </c>
     </row>
-    <row r="25" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="N25" t="s">
         <v>0</v>
       </c>
@@ -1500,7 +1540,7 @@
         <v>1.4623979978989561</v>
       </c>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>13</v>
       </c>
@@ -1553,7 +1593,7 @@
         <v>1.2652896258608302</v>
       </c>
     </row>
-    <row r="27" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B27">
         <f>$B$28*B29/1000</f>
         <v>5</v>
@@ -1649,7 +1689,7 @@
         <v>1.1580607939366052</v>
       </c>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>0</v>
       </c>
@@ -1707,7 +1747,7 @@
         <v>1.0149403497929366</v>
       </c>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -1765,7 +1805,7 @@
         <v>0.74</v>
       </c>
     </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>7</v>
       </c>
@@ -1823,7 +1863,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
       <c r="N31">
         <v>20</v>
       </c>
@@ -1845,7 +1885,7 @@
         <v>1.1599999999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B32">
         <f>$B$33*B34/1000</f>
         <v>0.5</v>
@@ -1911,7 +1951,7 @@
         <v>1.34</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>14</v>
       </c>
@@ -1939,7 +1979,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>0</v>
       </c>
@@ -1997,7 +2037,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>7</v>
       </c>
@@ -2055,7 +2095,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="N36">
         <v>4</v>
       </c>
@@ -2077,7 +2117,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="N37">
         <v>2</v>
       </c>
@@ -2099,7 +2139,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:20" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:20" ht="24" x14ac:dyDescent="0.25">
       <c r="N39" s="1" t="s">
         <v>16</v>
       </c>
@@ -2113,7 +2153,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="40" spans="1:20" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:20" ht="24" x14ac:dyDescent="0.25">
       <c r="N40" s="3" t="s">
         <v>18</v>
       </c>
@@ -2127,7 +2167,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="N41" s="3" t="s">
         <v>20</v>
       </c>
@@ -2141,71 +2181,71 @@
         <v>21</v>
       </c>
     </row>
-    <row r="42" spans="1:20" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="N42" s="3" t="s">
         <v>21</v>
       </c>
       <c r="O42" s="4" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="R42" s="3" t="s">
         <v>21</v>
       </c>
       <c r="S42" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="43" spans="1:20" ht="22.8" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" ht="24" x14ac:dyDescent="0.25">
       <c r="N43" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="O43" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="R43" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="S43" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" ht="48" x14ac:dyDescent="0.25">
+      <c r="N44" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="O43" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="R43" s="3" t="s">
+      <c r="O44" s="4">
+        <v>10684.813399999999</v>
+      </c>
+      <c r="R44" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="S43" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="44" spans="1:20" ht="34.200000000000003" x14ac:dyDescent="0.3">
-      <c r="N44" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="O44" s="4">
-        <v>71212.206839999999</v>
-      </c>
-      <c r="R44" s="3" t="s">
-        <v>25</v>
       </c>
       <c r="S44" s="4">
         <v>14837.657440000001</v>
       </c>
     </row>
-    <row r="45" spans="1:20" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:20" ht="60" x14ac:dyDescent="0.25">
       <c r="N45" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="O45" s="4">
-        <v>0.11873</v>
+        <v>0.62524000000000002</v>
       </c>
       <c r="R45" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="S45" s="4">
         <v>0.85443999999999998</v>
       </c>
     </row>
-    <row r="46" spans="1:20" ht="34.200000000000003" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="N46" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="O46" s="6">
-        <v>2.0809999999999999E-2</v>
+        <v>0.57840000000000003</v>
       </c>
       <c r="R46" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="S46" s="6">
         <v>0.83826999999999996</v>
@@ -2218,24 +2258,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
03: Small corrections, remade table 1
</commit_message>
<xml_diff>
--- a/03_PaschenuvZakon/data/PaschenuvZakon.xlsx
+++ b/03_PaschenuvZakon/data/PaschenuvZakon.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25028"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Desktop\Škola Mgr\Praktikum plazma\PraktikaPlazma\03_PaschenuvZakon\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{504E85C8-9CAB-4706-9D1D-3C3CB8F4E2E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="19176"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -34,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="56">
   <si>
     <t>Tlak [Pa]</t>
   </si>
@@ -148,14 +142,69 @@
   </si>
   <si>
     <t>1,0501 ± 0,02154</t>
+  </si>
+  <si>
+    <t>Měření s kontantním tlakem</t>
+  </si>
+  <si>
+    <t>Měření s konstantní vzdáleností elektrod</t>
+  </si>
+  <si>
+    <t>C'</t>
+  </si>
+  <si>
+    <t>Uz</t>
+  </si>
+  <si>
+    <t>pd</t>
+  </si>
+  <si>
+    <t>310 30</t>
+  </si>
+  <si>
+    <t>1.05 0.02</t>
+  </si>
+  <si>
+    <t>290 30</t>
+  </si>
+  <si>
+    <t>0.79 0.01</t>
+  </si>
+  <si>
+    <t>m2C-1</t>
+  </si>
+  <si>
+    <t>Pa</t>
+  </si>
+  <si>
+    <t>m2kgs-3A-1</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>kgm-1s-2</t>
+  </si>
+  <si>
+    <t>VPa-1m-1</t>
+  </si>
+  <si>
+    <t>m2s-1A-1</t>
+  </si>
+  <si>
+    <t>m2A-1s-1</t>
+  </si>
+  <si>
+    <t>Převody jednotek</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.00000000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -276,7 +325,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -297,9 +346,11 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normální" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -315,7 +366,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -357,7 +408,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -390,26 +441,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -442,23 +476,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -634,25 +651,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AE46"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AE55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="U45" sqref="U45"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="14" width="5.7109375" customWidth="1"/>
-    <col min="24" max="24" width="15.42578125" customWidth="1"/>
-    <col min="25" max="25" width="13.7109375" customWidth="1"/>
-    <col min="26" max="26" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="14" width="5.6640625" customWidth="1"/>
+    <col min="24" max="24" width="15.44140625" customWidth="1"/>
+    <col min="25" max="25" width="13.6640625" customWidth="1"/>
+    <col min="26" max="26" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -681,7 +698,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -713,7 +730,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -733,7 +750,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" ht="15" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>1</v>
       </c>
@@ -774,7 +791,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -818,7 +835,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -862,7 +879,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" ht="15" x14ac:dyDescent="0.25">
       <c r="Q7">
         <v>18</v>
       </c>
@@ -876,7 +893,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -896,7 +913,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -916,7 +933,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" ht="15" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>1</v>
       </c>
@@ -969,7 +986,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -1019,7 +1036,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -1069,7 +1086,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" ht="15" x14ac:dyDescent="0.25">
       <c r="W13">
         <v>7</v>
       </c>
@@ -1077,7 +1094,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" ht="15" x14ac:dyDescent="0.25">
       <c r="W14">
         <v>6</v>
       </c>
@@ -1085,7 +1102,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -1093,7 +1110,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -1125,7 +1142,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:31" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -1199,7 +1216,7 @@
         <v>3.4183012913197452</v>
       </c>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:31" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -1267,7 +1284,7 @@
         <v>3.0115704435972783</v>
       </c>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:31" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -1332,7 +1349,7 @@
         <v>2.6095944092252199</v>
       </c>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:31" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -1388,7 +1405,7 @@
         <v>2.4014005407815442</v>
       </c>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:31" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>11</v>
       </c>
@@ -1432,7 +1449,7 @@
         <v>2.2638726768652235</v>
       </c>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:31" ht="15" x14ac:dyDescent="0.25">
       <c r="X23">
         <f t="shared" si="1"/>
         <v>499.77119999999996</v>
@@ -1464,7 +1481,7 @@
         <v>2.0733517023869008</v>
       </c>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:31" ht="15" x14ac:dyDescent="0.25">
       <c r="X24">
         <f t="shared" si="1"/>
         <v>502.82379999999995</v>
@@ -1496,7 +1513,7 @@
         <v>1.8444771757456815</v>
       </c>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:31" ht="15" x14ac:dyDescent="0.25">
       <c r="N25" t="s">
         <v>0</v>
       </c>
@@ -1540,7 +1557,7 @@
         <v>1.4623979978989561</v>
       </c>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>13</v>
       </c>
@@ -1593,7 +1610,7 @@
         <v>1.2652896258608302</v>
       </c>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:31" ht="15" x14ac:dyDescent="0.25">
       <c r="B27">
         <f>$B$28*B29/1000</f>
         <v>5</v>
@@ -1689,7 +1706,7 @@
         <v>1.1580607939366052</v>
       </c>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:31" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>0</v>
       </c>
@@ -1747,7 +1764,7 @@
         <v>1.0149403497929366</v>
       </c>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:31" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -1805,7 +1822,7 @@
         <v>0.74</v>
       </c>
     </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>7</v>
       </c>
@@ -1863,7 +1880,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:31" ht="15" x14ac:dyDescent="0.25">
       <c r="N31">
         <v>20</v>
       </c>
@@ -1885,7 +1902,7 @@
         <v>1.1599999999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:31" ht="15" x14ac:dyDescent="0.25">
       <c r="B32">
         <f>$B$33*B34/1000</f>
         <v>0.5</v>
@@ -1951,7 +1968,7 @@
         <v>1.34</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>14</v>
       </c>
@@ -1979,7 +1996,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>0</v>
       </c>
@@ -2037,7 +2054,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>7</v>
       </c>
@@ -2095,7 +2112,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="N36">
         <v>4</v>
       </c>
@@ -2117,7 +2134,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="N37">
         <v>2</v>
       </c>
@@ -2167,7 +2184,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="N41" s="3" t="s">
         <v>20</v>
       </c>
@@ -2181,7 +2198,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="42" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" ht="22.8" x14ac:dyDescent="0.3">
       <c r="N42" s="3" t="s">
         <v>21</v>
       </c>
@@ -2195,7 +2212,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="43" spans="1:20" ht="24" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" ht="22.8" x14ac:dyDescent="0.3">
       <c r="N43" s="3" t="s">
         <v>22</v>
       </c>
@@ -2249,6 +2266,95 @@
       </c>
       <c r="S46" s="6">
         <v>0.83826999999999996</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B47" t="s">
+        <v>21</v>
+      </c>
+      <c r="C47" t="s">
+        <v>40</v>
+      </c>
+      <c r="D47" t="s">
+        <v>41</v>
+      </c>
+      <c r="E47" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A48" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B48" t="s">
+        <v>43</v>
+      </c>
+      <c r="C48" t="s">
+        <v>44</v>
+      </c>
+      <c r="D48" s="9">
+        <v>291.60000000000002</v>
+      </c>
+      <c r="E48">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B49" t="s">
+        <v>45</v>
+      </c>
+      <c r="C49" t="s">
+        <v>46</v>
+      </c>
+      <c r="D49" s="9">
+        <v>351.4</v>
+      </c>
+      <c r="E49">
+        <v>1.23</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" s="8"/>
+      <c r="D50" s="9"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>47</v>
+      </c>
+      <c r="B52" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B53" t="s">
+        <v>48</v>
+      </c>
+      <c r="C53" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B54" t="s">
+        <v>50</v>
+      </c>
+      <c r="C54" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>52</v>
+      </c>
+      <c r="B55" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -2258,24 +2364,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
03: Graph Corrections, v2
</commit_message>
<xml_diff>
--- a/03_PaschenuvZakon/data/PaschenuvZakon.xlsx
+++ b/03_PaschenuvZakon/data/PaschenuvZakon.xlsx
@@ -654,8 +654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M36" sqref="M36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1209,7 +1209,7 @@
       </c>
       <c r="AD18">
         <f t="shared" ref="AD18:AD27" si="0">AC18/$AC$28</f>
-        <v>0.51788722499499462</v>
+        <v>0.52387112331882535</v>
       </c>
       <c r="AE18">
         <f>LOG10(Z18)</f>
@@ -1277,7 +1277,7 @@
       </c>
       <c r="AD19">
         <f t="shared" si="0"/>
-        <v>0.59947719106602704</v>
+        <v>0.60640381598678927</v>
       </c>
       <c r="AE19">
         <f t="shared" ref="AE19:AE28" si="5">LOG10(Z19)</f>
@@ -1342,7 +1342,7 @@
       </c>
       <c r="AD20">
         <f t="shared" si="0"/>
-        <v>0.68011334440781535</v>
+        <v>0.68797167515087654</v>
       </c>
       <c r="AE20">
         <f t="shared" si="5"/>
@@ -1398,7 +1398,7 @@
       </c>
       <c r="AD21">
         <f t="shared" si="0"/>
-        <v>0.72187691055391512</v>
+        <v>0.73021779603360115</v>
       </c>
       <c r="AE21">
         <f t="shared" si="5"/>
@@ -1442,7 +1442,7 @@
       </c>
       <c r="AD22">
         <f t="shared" si="0"/>
-        <v>0.74946491823414574</v>
+        <v>0.75812456777084669</v>
       </c>
       <c r="AE22">
         <f t="shared" si="5"/>
@@ -1474,7 +1474,7 @@
       </c>
       <c r="AD23">
         <f t="shared" si="0"/>
-        <v>0.78768331236517874</v>
+        <v>0.79678455415120064</v>
       </c>
       <c r="AE23">
         <f t="shared" si="5"/>
@@ -1506,7 +1506,7 @@
       </c>
       <c r="AD24">
         <f t="shared" si="0"/>
-        <v>0.83359540624187134</v>
+        <v>0.84322713669093174</v>
       </c>
       <c r="AE24">
         <f t="shared" si="5"/>
@@ -1550,7 +1550,7 @@
       </c>
       <c r="AD25">
         <f t="shared" si="0"/>
-        <v>0.91024026200219399</v>
+        <v>0.92075758105390604</v>
       </c>
       <c r="AE25">
         <f t="shared" si="5"/>
@@ -1581,13 +1581,13 @@
       </c>
       <c r="X26">
         <f t="shared" si="1"/>
-        <v>551.43759999999997</v>
+        <v>492.01600000000002</v>
       </c>
       <c r="Y26">
         <v>15.72</v>
       </c>
       <c r="Z26">
-        <v>18.420000000000002</v>
+        <v>22.2</v>
       </c>
       <c r="AA26">
         <f t="shared" si="2"/>
@@ -1595,19 +1595,19 @@
       </c>
       <c r="AB26" s="7">
         <f t="shared" si="3"/>
-        <v>1.8420000000000003E-5</v>
+        <v>2.2200000000000001E-5</v>
       </c>
       <c r="AC26">
         <f t="shared" si="4"/>
-        <v>-4.7347103741391701</v>
+        <v>-4.6536470255493612</v>
       </c>
       <c r="AD26">
         <f t="shared" si="0"/>
-        <v>0.9497800841645907</v>
+        <v>0.94430511453836385</v>
       </c>
       <c r="AE26">
         <f t="shared" si="5"/>
-        <v>1.2652896258608302</v>
+        <v>1.3463529744506386</v>
       </c>
     </row>
     <row r="27" spans="1:31" ht="15" x14ac:dyDescent="0.25">
@@ -1677,13 +1677,13 @@
       </c>
       <c r="X27">
         <f t="shared" si="1"/>
-        <v>541.11239999999998</v>
+        <v>490.88799999999998</v>
       </c>
       <c r="Y27">
         <v>20.84</v>
       </c>
       <c r="Z27">
-        <v>14.39</v>
+        <v>16.8</v>
       </c>
       <c r="AA27">
         <f t="shared" si="2"/>
@@ -1691,19 +1691,19 @@
       </c>
       <c r="AB27" s="7">
         <f t="shared" si="3"/>
-        <v>1.4390000000000001E-5</v>
+        <v>1.6800000000000002E-5</v>
       </c>
       <c r="AC27">
         <f t="shared" si="4"/>
-        <v>-4.8419392060633948</v>
+        <v>-4.7746907182741367</v>
       </c>
       <c r="AD27">
         <f t="shared" si="0"/>
-        <v>0.97129012405343551</v>
+        <v>0.96886696409314876</v>
       </c>
       <c r="AE27">
         <f t="shared" si="5"/>
-        <v>1.1580607939366052</v>
+        <v>1.2253092817258628</v>
       </c>
     </row>
     <row r="28" spans="1:31" ht="15" x14ac:dyDescent="0.25">
@@ -1735,13 +1735,13 @@
       </c>
       <c r="X28">
         <f t="shared" si="1"/>
-        <v>530.29300000000001</v>
+        <v>486.76400000000001</v>
       </c>
       <c r="Y28">
         <v>30.02</v>
       </c>
       <c r="Z28">
-        <v>10.35</v>
+        <v>11.8</v>
       </c>
       <c r="AA28">
         <f t="shared" si="2"/>
@@ -1749,11 +1749,11 @@
       </c>
       <c r="AB28" s="7">
         <f t="shared" si="3"/>
-        <v>1.0349999999999999E-5</v>
+        <v>1.1800000000000001E-5</v>
       </c>
       <c r="AC28">
         <f t="shared" si="4"/>
-        <v>-4.9850596502070639</v>
+        <v>-4.928117992693875</v>
       </c>
       <c r="AD28">
         <f>AC28/$AC$28</f>
@@ -1761,7 +1761,7 @@
       </c>
       <c r="AE28">
         <f t="shared" si="5"/>
-        <v>1.0149403497929366</v>
+        <v>1.0718820073061255</v>
       </c>
     </row>
     <row r="29" spans="1:31" ht="15" x14ac:dyDescent="0.25">
@@ -1900,6 +1900,22 @@
       <c r="T31">
         <f t="shared" si="8"/>
         <v>1.1599999999999999</v>
+      </c>
+      <c r="W31">
+        <f>LOG10(P27)</f>
+        <v>0.69897000433601886</v>
+      </c>
+      <c r="X31">
+        <f>LOG10(O27)</f>
+        <v>2.6532125137753435</v>
+      </c>
+      <c r="Z31">
+        <f>LOG10(T27)</f>
+        <v>-0.3010299956639812</v>
+      </c>
+      <c r="AA31">
+        <f>LOG10(S27)</f>
+        <v>3.1335389083702174</v>
       </c>
     </row>
     <row r="32" spans="1:31" ht="15" x14ac:dyDescent="0.25">
@@ -1967,8 +1983,24 @@
         <f t="shared" si="8"/>
         <v>1.34</v>
       </c>
-    </row>
-    <row r="33" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+      <c r="W32">
+        <f t="shared" ref="W32:W41" si="10">LOG10(P28)</f>
+        <v>0.6020599913279624</v>
+      </c>
+      <c r="X32">
+        <f t="shared" ref="X32:X41" si="11">LOG10(O28)</f>
+        <v>2.6334684555795866</v>
+      </c>
+      <c r="Z32">
+        <f t="shared" ref="Z32:Z41" si="12">LOG10(T28)</f>
+        <v>-0.22184874961635639</v>
+      </c>
+      <c r="AA32">
+        <f t="shared" ref="AA32:AA41" si="13">LOG10(S28)</f>
+        <v>2.9294189257142929</v>
+      </c>
+    </row>
+    <row r="33" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>14</v>
       </c>
@@ -1995,8 +2027,24 @@
         <f t="shared" si="8"/>
         <v>1.6</v>
       </c>
-    </row>
-    <row r="34" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+      <c r="W33">
+        <f t="shared" si="10"/>
+        <v>0.47712125471966244</v>
+      </c>
+      <c r="X33">
+        <f t="shared" si="11"/>
+        <v>2.5910646070264991</v>
+      </c>
+      <c r="Z33">
+        <f t="shared" si="12"/>
+        <v>-0.13076828026902382</v>
+      </c>
+      <c r="AA33">
+        <f t="shared" si="13"/>
+        <v>2.7481880270062002</v>
+      </c>
+    </row>
+    <row r="34" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>0</v>
       </c>
@@ -2053,8 +2101,24 @@
         <f t="shared" si="8"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="W34">
+        <f t="shared" si="10"/>
+        <v>0.3979400086720376</v>
+      </c>
+      <c r="X34">
+        <f t="shared" si="11"/>
+        <v>2.5797835966168101</v>
+      </c>
+      <c r="Z34">
+        <f t="shared" si="12"/>
+        <v>-3.6212172654444715E-2</v>
+      </c>
+      <c r="AA34">
+        <f t="shared" si="13"/>
+        <v>2.6627578316815739</v>
+      </c>
+    </row>
+    <row r="35" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>7</v>
       </c>
@@ -2111,8 +2175,24 @@
         <f t="shared" si="8"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="36" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+      <c r="W35">
+        <f t="shared" si="10"/>
+        <v>0.3010299956639812</v>
+      </c>
+      <c r="X35">
+        <f t="shared" si="11"/>
+        <v>2.5563025007672873</v>
+      </c>
+      <c r="Z35">
+        <f t="shared" si="12"/>
+        <v>6.445798922691845E-2</v>
+      </c>
+      <c r="AA35">
+        <f t="shared" si="13"/>
+        <v>2.6127838567197355</v>
+      </c>
+    </row>
+    <row r="36" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="N36">
         <v>4</v>
       </c>
@@ -2133,8 +2213,24 @@
         <f t="shared" si="8"/>
         <v>4.4000000000000004</v>
       </c>
-    </row>
-    <row r="37" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+      <c r="W36">
+        <f t="shared" si="10"/>
+        <v>0.17609125905568124</v>
+      </c>
+      <c r="X36">
+        <f t="shared" si="11"/>
+        <v>2.568201724066995</v>
+      </c>
+      <c r="Z36">
+        <f t="shared" si="12"/>
+        <v>0.12710479836480765</v>
+      </c>
+      <c r="AA36">
+        <f t="shared" si="13"/>
+        <v>2.5797835966168101</v>
+      </c>
+    </row>
+    <row r="37" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="N37">
         <v>2</v>
       </c>
@@ -2155,8 +2251,42 @@
         <f t="shared" si="8"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="39" spans="1:20" ht="24" x14ac:dyDescent="0.25">
+      <c r="W37">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="X37">
+        <f t="shared" si="11"/>
+        <v>2.6020599913279625</v>
+      </c>
+      <c r="Z37">
+        <f t="shared" si="12"/>
+        <v>0.20411998265592479</v>
+      </c>
+      <c r="AA37">
+        <f t="shared" si="13"/>
+        <v>2.568201724066995</v>
+      </c>
+    </row>
+    <row r="38" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="W38">
+        <f t="shared" si="10"/>
+        <v>-4.5757490560675115E-2</v>
+      </c>
+      <c r="X38">
+        <f t="shared" si="11"/>
+        <v>2.6434526764861874</v>
+      </c>
+      <c r="Z38">
+        <f t="shared" si="12"/>
+        <v>0.3010299956639812</v>
+      </c>
+      <c r="AA38">
+        <f t="shared" si="13"/>
+        <v>2.5563025007672873</v>
+      </c>
+    </row>
+    <row r="39" spans="1:27" ht="24" x14ac:dyDescent="0.25">
       <c r="N39" s="1" t="s">
         <v>16</v>
       </c>
@@ -2169,8 +2299,24 @@
       <c r="S39" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="40" spans="1:20" ht="24" x14ac:dyDescent="0.25">
+      <c r="W39">
+        <f t="shared" si="10"/>
+        <v>-0.15490195998574319</v>
+      </c>
+      <c r="X39">
+        <f t="shared" si="11"/>
+        <v>2.6720978579357175</v>
+      </c>
+      <c r="Z39">
+        <f t="shared" si="12"/>
+        <v>0.47712125471966244</v>
+      </c>
+      <c r="AA39">
+        <f t="shared" si="13"/>
+        <v>2.5797835966168101</v>
+      </c>
+    </row>
+    <row r="40" spans="1:27" ht="24" x14ac:dyDescent="0.25">
       <c r="N40" s="3" t="s">
         <v>18</v>
       </c>
@@ -2183,8 +2329,24 @@
       <c r="S40" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="41" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+      <c r="W40">
+        <f t="shared" si="10"/>
+        <v>-0.3979400086720376</v>
+      </c>
+      <c r="X40">
+        <f t="shared" si="11"/>
+        <v>2.9542425094393248</v>
+      </c>
+      <c r="Z40">
+        <f t="shared" si="12"/>
+        <v>0.64345267648618742</v>
+      </c>
+      <c r="AA40">
+        <f t="shared" si="13"/>
+        <v>2.6232492903979003</v>
+      </c>
+    </row>
+    <row r="41" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="N41" s="3" t="s">
         <v>20</v>
       </c>
@@ -2197,8 +2359,24 @@
       <c r="S41" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="42" spans="1:20" ht="22.8" x14ac:dyDescent="0.3">
+      <c r="W41">
+        <f t="shared" si="10"/>
+        <v>-0.69897000433601875</v>
+      </c>
+      <c r="X41">
+        <f t="shared" si="11"/>
+        <v>3.0791812460476247</v>
+      </c>
+      <c r="Z41">
+        <f t="shared" si="12"/>
+        <v>0.77815125038364363</v>
+      </c>
+      <c r="AA41">
+        <f t="shared" si="13"/>
+        <v>2.7242758696007892</v>
+      </c>
+    </row>
+    <row r="42" spans="1:27" ht="22.8" x14ac:dyDescent="0.3">
       <c r="N42" s="3" t="s">
         <v>21</v>
       </c>
@@ -2212,7 +2390,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="43" spans="1:20" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:27" ht="22.8" x14ac:dyDescent="0.3">
       <c r="N43" s="3" t="s">
         <v>22</v>
       </c>
@@ -2226,7 +2404,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="44" spans="1:20" ht="48" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:27" ht="48" x14ac:dyDescent="0.25">
       <c r="N44" s="3" t="s">
         <v>23</v>
       </c>
@@ -2240,7 +2418,7 @@
         <v>14837.657440000001</v>
       </c>
     </row>
-    <row r="45" spans="1:20" ht="60" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:27" ht="60" x14ac:dyDescent="0.25">
       <c r="N45" s="3" t="s">
         <v>24</v>
       </c>
@@ -2254,7 +2432,7 @@
         <v>0.85443999999999998</v>
       </c>
     </row>
-    <row r="46" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:27" ht="36" x14ac:dyDescent="0.25">
       <c r="N46" s="5" t="s">
         <v>25</v>
       </c>
@@ -2268,7 +2446,7 @@
         <v>0.83826999999999996</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
         <v>21</v>
       </c>
@@ -2282,7 +2460,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A48" s="8" t="s">
         <v>38</v>
       </c>

</xml_diff>

<commit_message>
01; 03: Origin Kudrle
</commit_message>
<xml_diff>
--- a/03_PaschenuvZakon/data/PaschenuvZakon.xlsx
+++ b/03_PaschenuvZakon/data/PaschenuvZakon.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="19176"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -654,22 +654,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M36" sqref="M36"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="W36" sqref="W36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="14" width="5.6640625" customWidth="1"/>
-    <col min="24" max="24" width="15.44140625" customWidth="1"/>
-    <col min="25" max="25" width="13.6640625" customWidth="1"/>
-    <col min="26" max="26" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="14" width="5.7109375" customWidth="1"/>
+    <col min="24" max="24" width="15.42578125" customWidth="1"/>
+    <col min="25" max="25" width="13.7109375" customWidth="1"/>
+    <col min="26" max="26" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -698,7 +698,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -730,7 +730,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -750,7 +750,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="4" spans="1:24" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>1</v>
       </c>
@@ -791,7 +791,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="5" spans="1:24" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -835,7 +835,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="6" spans="1:24" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -879,7 +879,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="7" spans="1:24" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="Q7">
         <v>18</v>
       </c>
@@ -893,7 +893,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="8" spans="1:24" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -913,7 +913,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="9" spans="1:24" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -933,7 +933,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="10" spans="1:24" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>1</v>
       </c>
@@ -986,7 +986,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="11" spans="1:24" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -1036,7 +1036,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="12" spans="1:24" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -1086,7 +1086,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="13" spans="1:24" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="W13">
         <v>7</v>
       </c>
@@ -1094,7 +1094,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="14" spans="1:24" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="W14">
         <v>6</v>
       </c>
@@ -1102,7 +1102,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="16" spans="1:24" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -1110,7 +1110,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -1142,7 +1142,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -1216,7 +1216,7 @@
         <v>3.4183012913197452</v>
       </c>
     </row>
-    <row r="19" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -1284,7 +1284,7 @@
         <v>3.0115704435972783</v>
       </c>
     </row>
-    <row r="20" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -1349,7 +1349,7 @@
         <v>2.6095944092252199</v>
       </c>
     </row>
-    <row r="21" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -1405,7 +1405,7 @@
         <v>2.4014005407815442</v>
       </c>
     </row>
-    <row r="22" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>11</v>
       </c>
@@ -1449,7 +1449,7 @@
         <v>2.2638726768652235</v>
       </c>
     </row>
-    <row r="23" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="X23">
         <f t="shared" si="1"/>
         <v>499.77119999999996</v>
@@ -1481,7 +1481,7 @@
         <v>2.0733517023869008</v>
       </c>
     </row>
-    <row r="24" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="X24">
         <f t="shared" si="1"/>
         <v>502.82379999999995</v>
@@ -1513,7 +1513,7 @@
         <v>1.8444771757456815</v>
       </c>
     </row>
-    <row r="25" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="N25" t="s">
         <v>0</v>
       </c>
@@ -1557,7 +1557,7 @@
         <v>1.4623979978989561</v>
       </c>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>13</v>
       </c>
@@ -1610,7 +1610,7 @@
         <v>1.3463529744506386</v>
       </c>
     </row>
-    <row r="27" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B27">
         <f>$B$28*B29/1000</f>
         <v>5</v>
@@ -1706,7 +1706,7 @@
         <v>1.2253092817258628</v>
       </c>
     </row>
-    <row r="28" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>0</v>
       </c>
@@ -1764,7 +1764,7 @@
         <v>1.0718820073061255</v>
       </c>
     </row>
-    <row r="29" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -1822,7 +1822,7 @@
         <v>0.74</v>
       </c>
     </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>7</v>
       </c>
@@ -1880,7 +1880,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="31" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
       <c r="N31">
         <v>20</v>
       </c>
@@ -1918,7 +1918,7 @@
         <v>3.1335389083702174</v>
       </c>
     </row>
-    <row r="32" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B32">
         <f>$B$33*B34/1000</f>
         <v>0.5</v>
@@ -2000,7 +2000,7 @@
         <v>2.9294189257142929</v>
       </c>
     </row>
-    <row r="33" spans="1:27" ht="15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>14</v>
       </c>
@@ -2044,7 +2044,7 @@
         <v>2.7481880270062002</v>
       </c>
     </row>
-    <row r="34" spans="1:27" ht="15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>0</v>
       </c>
@@ -2118,7 +2118,7 @@
         <v>2.6627578316815739</v>
       </c>
     </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>7</v>
       </c>
@@ -2192,7 +2192,7 @@
         <v>2.6127838567197355</v>
       </c>
     </row>
-    <row r="36" spans="1:27" ht="15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
       <c r="N36">
         <v>4</v>
       </c>
@@ -2230,7 +2230,7 @@
         <v>2.5797835966168101</v>
       </c>
     </row>
-    <row r="37" spans="1:27" ht="15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
       <c r="N37">
         <v>2</v>
       </c>
@@ -2268,7 +2268,7 @@
         <v>2.568201724066995</v>
       </c>
     </row>
-    <row r="38" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:27" ht="14.45" x14ac:dyDescent="0.3">
       <c r="W38">
         <f t="shared" si="10"/>
         <v>-4.5757490560675115E-2</v>
@@ -2346,7 +2346,7 @@
         <v>2.6232492903979003</v>
       </c>
     </row>
-    <row r="41" spans="1:27" ht="15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
       <c r="N41" s="3" t="s">
         <v>20</v>
       </c>
@@ -2376,7 +2376,7 @@
         <v>2.7242758696007892</v>
       </c>
     </row>
-    <row r="42" spans="1:27" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:27" ht="36" x14ac:dyDescent="0.25">
       <c r="N42" s="3" t="s">
         <v>21</v>
       </c>
@@ -2390,7 +2390,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="43" spans="1:27" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:27" ht="24" x14ac:dyDescent="0.25">
       <c r="N43" s="3" t="s">
         <v>22</v>
       </c>
@@ -2402,6 +2402,10 @@
       </c>
       <c r="S43" s="4" t="s">
         <v>27</v>
+      </c>
+      <c r="V43">
+        <f>EXP(-0.4)</f>
+        <v>0.67032004603563933</v>
       </c>
     </row>
     <row r="44" spans="1:27" ht="48" x14ac:dyDescent="0.25">
@@ -2446,7 +2450,7 @@
         <v>0.83826999999999996</v>
       </c>
     </row>
-    <row r="47" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>21</v>
       </c>
@@ -2460,7 +2464,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="48" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
         <v>38</v>
       </c>
@@ -2477,7 +2481,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
         <v>39</v>
       </c>
@@ -2494,16 +2498,16 @@
         <v>1.23</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="8"/>
       <c r="D50" s="9"/>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>47</v>
       </c>
@@ -2511,7 +2515,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>48</v>
       </c>
@@ -2519,7 +2523,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>50</v>
       </c>
@@ -2527,7 +2531,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>52</v>
       </c>
@@ -2547,7 +2551,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2559,7 +2563,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>